<commit_message>
Update on employee template
</commit_message>
<xml_diff>
--- a/public/employeetemplate2.xlsx
+++ b/public/employeetemplate2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\__scorpion_\Desktop\New folder\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE4E7B9-C4E2-4FC8-BEC0-87EDF72AEEA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED316C13-06D0-4F60-90CE-5D1B2F6A0E18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{0F0D9703-A8B6-4853-94FD-6DD23239D8D1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>firstName</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>zipcode</t>
-  </si>
-  <si>
-    <t>street</t>
   </si>
   <si>
     <t>phone</t>
@@ -99,24 +96,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -132,16 +123,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC0021A5-8F53-436E-83EE-78275247535D}" name="Table1" displayName="Table1" ref="A1:J8" totalsRowShown="0">
-  <autoFilter ref="A1:J8" xr:uid="{843926C8-ABF4-4332-9CE1-95392F69B600}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC0021A5-8F53-436E-83EE-78275247535D}" name="Table1" displayName="Table1" ref="A1:I8" totalsRowShown="0">
+  <autoFilter ref="A1:I8" xr:uid="{843926C8-ABF4-4332-9CE1-95392F69B600}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8E9FEFD-E446-4974-8465-922E1AB5E54B}" name="firstName"/>
     <tableColumn id="2" xr3:uid="{ED00BE51-6FC7-4B02-B1AD-708C6A9F007A}" name="lastName"/>
     <tableColumn id="3" xr3:uid="{DC3A3FD4-4073-4C7C-89C0-68C0E1B39D56}" name="email"/>
     <tableColumn id="4" xr3:uid="{D43BB35A-80D9-4A17-836C-1782CEFC2C50}" name="state"/>
     <tableColumn id="5" xr3:uid="{70A9E2AB-C61A-4220-B6DE-F4852412DD4B}" name="city"/>
     <tableColumn id="6" xr3:uid="{3F0AA410-02EE-46BB-B987-E375A9D2D002}" name="zipcode"/>
-    <tableColumn id="7" xr3:uid="{4E31875C-FC4E-4BEF-AB70-5AA60B42A815}" name="street" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{371299E9-5E43-41E8-ADA7-BE722805719D}" name="phone" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{185D35C0-93FD-4DE9-9F6B-49660B8976B4}" name="role"/>
     <tableColumn id="10" xr3:uid="{719A3650-CF68-49BD-BD6F-EED15FE4FE55}" name="password"/>
@@ -447,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEAF63C0-C729-4140-B081-231DD78E86D4}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,13 +451,12 @@
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25" style="3" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="25" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,22 +478,19 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{EE3E8AB6-3F37-456A-AC2D-A5582656FAFB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{EE3E8AB6-3F37-456A-AC2D-A5582656FAFB}">
       <formula1>"dispatcher, technician, business admin"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>